<commit_message>
removing inconsistent to maze architecture in door in 222, was just extra
</commit_message>
<xml_diff>
--- a/cube_mazes/26.xlsx
+++ b/cube_mazes/26.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javascript_Misc\maze_messing_1\cube_mazes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9802B432-FFDE-42A7-8BB8-D0C7D03481F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DCC5B8-DCC8-4D5D-822D-C70C1F042DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="4">
   <si>
     <t>X</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -177,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +360,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -524,9 +527,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,7 +900,7 @@
   <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,8 +3773,8 @@
       <c r="AA27" t="s">
         <v>0</v>
       </c>
-      <c r="AB27" s="1" t="s">
-        <v>4</v>
+      <c r="AB27" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="AC27" t="s">
         <v>0</v>

</xml_diff>